<commit_message>
fix: newline for row spacing
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ben\projects\Planning-Inspectorate\ddat-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BD81CC4-36D7-4A03-ACC3-937B8B905095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD774F1C-571E-4C3D-9B04-5CC5132FCF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1275" windowWidth="24960" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Assessment" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
   <si>
     <r>
       <rPr>
@@ -170,9 +170,6 @@
     <t>Job family:</t>
   </si>
   <si>
-    <t>Software Development</t>
-  </si>
-  <si>
     <t>Date discussed with Line Manager</t>
   </si>
   <si>
@@ -182,19 +179,10 @@
     <t>Role:</t>
   </si>
   <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
     <t>Enter a date in the format DD/MM/YYYY</t>
   </si>
   <si>
-    <t>5. Send this completed spreadsheet and any supporting documents (in PDF format where possible) as attachments to the email address below:</t>
-  </si>
-  <si>
     <t>Role-level:</t>
-  </si>
-  <si>
-    <t>Lead Developer (Management)</t>
   </si>
   <si>
     <t>Skills</t>
@@ -329,130 +317,6 @@
       </rPr>
       <t>List the filenames of any anonymised documents you wish to use as supporting evidence. Ensure documents with the correct filenames are attached in the same email you use to submit this completed spreadsheet. Do not insert links or embed files in this spreadsheet.</t>
     </r>
-  </si>
-  <si>
-    <t>Availability and capacity management</t>
-  </si>
-  <si>
-    <t>Availability and capacity management involves ensuring services are available with as little down-time or disruption as possible, whilst making sure we have sufficient resources to support emerging business needs.</t>
-  </si>
-  <si>
-    <t>Practitioner</t>
-  </si>
-  <si>
-    <t>You can:
-- ensure the correct implementation of standards and procedures
-- identify capacity issues, and stipulate and instigate the required changes
-initiate remedial action</t>
-  </si>
-  <si>
-    <t>Development process optimisation</t>
-  </si>
-  <si>
-    <t>Process optimisation involves ensuring your processes are accurately defined and capture the most efficient way to complete a task by monitoring modified procedures.</t>
-  </si>
-  <si>
-    <t>You can:
-- analyse current processes
-- identify and implement opportunities to optimise processes
-- lead and develop a team of experts to deliver service improvements
-- help to evaluate and establish requirements for the implementation of changes by setting policy and standards</t>
-  </si>
-  <si>
-    <t>Information security</t>
-  </si>
-  <si>
-    <t>Information security involves maintaining the security, confidentiality and integrity of information.</t>
-  </si>
-  <si>
-    <t>You can:
-- understand information security
-- design solutions and services with security controls embedded, specifically engineered with mitigation of security threats as a core feature</t>
-  </si>
-  <si>
-    <t>Modern standards approach</t>
-  </si>
-  <si>
-    <t>Modern development standards involves using the latest technologies and best practices to improve the quality of the software development process.</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>You can:
-- demonstrate a strong understanding of the most appropriate modern standards and practices, and how they are applied
-- coach and guide others in these standards</t>
-  </si>
-  <si>
-    <t>Programming and build (software engineering)</t>
-  </si>
-  <si>
-    <t>You can use agreed security standards and specifications to design, create, test and document new or amended software.</t>
-  </si>
-  <si>
-    <t>You can:
-- collaborate with others when necessary to review specifications
-- use the agreed specifications to design, code, test and document programs or scripts of medium-to-high complexity, using the right standards and tools</t>
-  </si>
-  <si>
-    <t>Prototyping</t>
-  </si>
-  <si>
-    <t>Prototyping a service or product involves exploring, testing and sharing different concepts before committing to the final design.</t>
-  </si>
-  <si>
-    <t>You can:
-- approach prototyping as a team activity, actively soliciting prototypes and testing with others
-- establish design patterns and iterate them
-- use a variety of prototyping methods and choose the most appropriate</t>
-  </si>
-  <si>
-    <t>Service support</t>
-  </si>
-  <si>
-    <t>Service support involves fixing service faults and maintaining the underlying infrastructure, ensuring processes are in place to keep the service running efficiently.</t>
-  </si>
-  <si>
-    <t>You can:
-- identify, locate and fix faults</t>
-  </si>
-  <si>
-    <t>Systems design</t>
-  </si>
-  <si>
-    <t>Systems design involves creating the specification and design of systems to meet defined business needs.</t>
-  </si>
-  <si>
-    <t>You can:
-- design systems characterised by medium levels of risk, impact, and business or technical complexity
-- select appropriate design standards, methods and tools, and ensure they are applied effectively
-- review the systems designs of others to ensure the selection of appropriate technology, efficient use of resources and integration of multiple systems and technology</t>
-  </si>
-  <si>
-    <t>Systems integration</t>
-  </si>
-  <si>
-    <t>Systems integration involves identifying points of connection between different systems and processes, or opportunities to combine them, and designing how the components communicate.</t>
-  </si>
-  <si>
-    <t>You can:
-- define the integration build
-- co-ordinate build activities across systems
-- understand how to undertake and support integration testing activities</t>
-  </si>
-  <si>
-    <t>User focus</t>
-  </si>
-  <si>
-    <t>User focus involves understanding the user needs to develop a detailed understanding of the problems that need to be solved.</t>
-  </si>
-  <si>
-    <t>You can:
-- collaborate with user researchers and can represent users internally
-- explain the difference between user needs and the desires of the user
-- champion user research to focus on all users
-- prioritise and define approaches to understand the user story, guiding others in doing so
-- offer recommendations on the best tools and methods to use</t>
   </si>
   <si>
     <t>Evaluation Sheet</t>
@@ -738,6 +602,9 @@
   </si>
   <si>
     <t>Moderator Comments:</t>
+  </si>
+  <si>
+    <t>5. Email this completed spreadsheet and any supporting documents (in PDF format where possible) as attachments to your Head of Service (Head of Digital or Head of Data)</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +1905,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2202,16 +2069,14 @@
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="C11" s="16"/>
       <c r="D11" s="17"/>
       <c r="E11" s="149" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -2220,18 +2085,16 @@
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="17"/>
       <c r="E12" s="151" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -2240,17 +2103,13 @@
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="152" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="153" t="s">
-        <v>20</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C13" s="153"/>
       <c r="D13" s="17"/>
       <c r="E13" s="20"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="178" t="s">
-        <v>6</v>
-      </c>
+      <c r="G13" s="178"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="1"/>
@@ -2270,14 +2129,14 @@
     <row r="15" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="180" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15" s="181"/>
       <c r="D15" s="181"/>
       <c r="E15" s="182"/>
       <c r="F15" s="154"/>
       <c r="G15" s="183" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H15" s="181"/>
       <c r="I15" s="182"/>
@@ -2286,223 +2145,143 @@
     <row r="16" spans="1:10" ht="104" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F16" s="154"/>
       <c r="G16" s="24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="100" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
-      <c r="B17" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>33</v>
-      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="154"/>
       <c r="G17" s="30"/>
       <c r="H17" s="179"/>
       <c r="I17" s="179"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="125" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
-      <c r="B18" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="154"/>
       <c r="G18" s="30"/>
       <c r="H18" s="179"/>
       <c r="I18" s="31"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="87.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
-      <c r="B19" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>39</v>
-      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="154"/>
       <c r="G19" s="30"/>
       <c r="H19" s="179"/>
       <c r="I19" s="179"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="87.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
-      <c r="B20" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>43</v>
-      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="154"/>
       <c r="G20" s="30"/>
       <c r="H20" s="179"/>
       <c r="I20" s="179"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
-      <c r="B21" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>46</v>
-      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="154"/>
       <c r="G21" s="30"/>
       <c r="H21" s="179"/>
       <c r="I21" s="179"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
-      <c r="B22" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>49</v>
-      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="154"/>
       <c r="G22" s="30"/>
       <c r="H22" s="179"/>
       <c r="I22" s="31"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
-      <c r="B23" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>52</v>
-      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="154"/>
       <c r="G23" s="30"/>
       <c r="H23" s="179"/>
       <c r="I23" s="31"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
-      <c r="B24" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>55</v>
-      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="154"/>
       <c r="G24" s="30"/>
       <c r="H24" s="179"/>
       <c r="I24" s="179"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="87.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
-      <c r="B25" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>58</v>
-      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="154"/>
       <c r="G25" s="30"/>
       <c r="H25" s="179"/>
       <c r="I25" s="179"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="162.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="177" t="s">
-        <v>61</v>
-      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="177"/>
       <c r="F26" s="154"/>
       <c r="G26" s="30"/>
       <c r="H26" s="179"/>
@@ -2533,11 +2312,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{59C13787-7B29-4E3C-BCE2-4FD52A40DBC7}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{5FA93F4D-493B-45CA-BB60-36363FBFE524}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="8" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId3"/>
+  <pageSetup paperSize="8" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL&amp;1#_x000D_</oddHeader>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL</oddFooter>
@@ -2645,12 +2423,12 @@
     <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="37"/>
       <c r="B4" s="41" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="49"/>
       <c r="E4" s="155" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -2711,13 +2489,13 @@
       <c r="B7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="16" t="str">
+      <c r="C7" s="16">
         <f>('Self-Assessment'!C11)</f>
-        <v>Software Development</v>
+        <v>0</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="155" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="54"/>
@@ -2729,18 +2507,18 @@
       <c r="M7" s="54"/>
       <c r="N7" s="54"/>
       <c r="O7" s="157" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="P7" s="39"/>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
       <c r="B8" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="str">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19">
         <f>('Self-Assessment'!C12)</f>
-        <v>Software Developer</v>
+        <v>0</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="158"/>
@@ -2754,18 +2532,18 @@
       <c r="M8" s="56"/>
       <c r="N8" s="56"/>
       <c r="O8" s="151" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="42"/>
       <c r="B9" s="159" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="153" t="str">
+        <v>16</v>
+      </c>
+      <c r="C9" s="153">
         <f>('Self-Assessment'!C13)</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="57">
@@ -2823,7 +2601,7 @@
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="180" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12" s="181"/>
       <c r="D12" s="181"/>
@@ -2832,12 +2610,12 @@
       <c r="G12" s="184"/>
       <c r="H12" s="181"/>
       <c r="I12" s="183" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J12" s="182"/>
       <c r="K12" s="42"/>
       <c r="L12" s="180" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="M12" s="181"/>
       <c r="N12" s="181"/>
@@ -2847,65 +2625,62 @@
     <row r="13" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="22" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" s="160"/>
       <c r="G13" s="61" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="K13" s="42"/>
       <c r="L13" s="22" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="P13" s="42"/>
     </row>
     <row r="14" spans="1:16" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
-      <c r="B14" s="26" t="str">
+      <c r="B14" s="26">
         <f>('Self-Assessment'!B17)</f>
-        <v>Availability and capacity management</v>
-      </c>
-      <c r="C14" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C14" s="27">
         <f>('Self-Assessment'!C17)</f>
-        <v>Availability and capacity management involves ensuring services are available with as little down-time or disruption as possible, whilst making sure we have sufficient resources to support emerging business needs.</v>
-      </c>
-      <c r="D14" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28">
         <f>('Self-Assessment'!D17)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E14" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29">
         <f>('Self-Assessment'!E17)</f>
-        <v>You can:
-- ensure the correct implementation of standards and procedures
-- identify capacity issues, and stipulate and instigate the required changes
-initiate remedial action</v>
+        <v>0</v>
       </c>
       <c r="F14" s="160"/>
       <c r="G14" s="63">
@@ -2939,25 +2714,21 @@
     </row>
     <row r="15" spans="1:16" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="62"/>
-      <c r="B15" s="26" t="str">
+      <c r="B15" s="26">
         <f>('Self-Assessment'!B18)</f>
-        <v>Development process optimisation</v>
-      </c>
-      <c r="C15" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C15" s="27">
         <f>('Self-Assessment'!C18)</f>
-        <v>Process optimisation involves ensuring your processes are accurately defined and capture the most efficient way to complete a task by monitoring modified procedures.</v>
-      </c>
-      <c r="D15" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28">
         <f>('Self-Assessment'!D18)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E15" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
         <f>('Self-Assessment'!E18)</f>
-        <v>You can:
-- analyse current processes
-- identify and implement opportunities to optimise processes
-- lead and develop a team of experts to deliver service improvements
-- help to evaluate and establish requirements for the implementation of changes by setting policy and standards</v>
+        <v>0</v>
       </c>
       <c r="F15" s="160"/>
       <c r="G15" s="63">
@@ -2991,23 +2762,21 @@
     </row>
     <row r="16" spans="1:16" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="62"/>
-      <c r="B16" s="26" t="str">
+      <c r="B16" s="26">
         <f>('Self-Assessment'!B19)</f>
-        <v>Information security</v>
-      </c>
-      <c r="C16" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27">
         <f>('Self-Assessment'!C19)</f>
-        <v>Information security involves maintaining the security, confidentiality and integrity of information.</v>
-      </c>
-      <c r="D16" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28">
         <f>('Self-Assessment'!D19)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E16" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29">
         <f>('Self-Assessment'!E19)</f>
-        <v>You can:
-- understand information security
-- design solutions and services with security controls embedded, specifically engineered with mitigation of security threats as a core feature</v>
+        <v>0</v>
       </c>
       <c r="F16" s="160"/>
       <c r="G16" s="63">
@@ -3041,23 +2810,21 @@
     </row>
     <row r="17" spans="1:16" ht="291" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62"/>
-      <c r="B17" s="26" t="str">
+      <c r="B17" s="26">
         <f>('Self-Assessment'!B20)</f>
-        <v>Modern standards approach</v>
-      </c>
-      <c r="C17" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C17" s="27">
         <f>('Self-Assessment'!C20)</f>
-        <v>Modern development standards involves using the latest technologies and best practices to improve the quality of the software development process.</v>
-      </c>
-      <c r="D17" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D17" s="28">
         <f>('Self-Assessment'!D20)</f>
-        <v>Expert</v>
-      </c>
-      <c r="E17" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E17" s="29">
         <f>('Self-Assessment'!E20)</f>
-        <v>You can:
-- demonstrate a strong understanding of the most appropriate modern standards and practices, and how they are applied
-- coach and guide others in these standards</v>
+        <v>0</v>
       </c>
       <c r="F17" s="160"/>
       <c r="G17" s="63">
@@ -3091,23 +2858,21 @@
     </row>
     <row r="18" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
-      <c r="B18" s="26" t="str">
+      <c r="B18" s="26">
         <f>('Self-Assessment'!B21)</f>
-        <v>Programming and build (software engineering)</v>
-      </c>
-      <c r="C18" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C18" s="27">
         <f>('Self-Assessment'!C21)</f>
-        <v>You can use agreed security standards and specifications to design, create, test and document new or amended software.</v>
-      </c>
-      <c r="D18" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D18" s="28">
         <f>('Self-Assessment'!D21)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E18" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E18" s="29">
         <f>('Self-Assessment'!E21)</f>
-        <v>You can:
-- collaborate with others when necessary to review specifications
-- use the agreed specifications to design, code, test and document programs or scripts of medium-to-high complexity, using the right standards and tools</v>
+        <v>0</v>
       </c>
       <c r="F18" s="160"/>
       <c r="G18" s="63">
@@ -3141,24 +2906,21 @@
     </row>
     <row r="19" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62"/>
-      <c r="B19" s="26" t="str">
+      <c r="B19" s="26">
         <f>('Self-Assessment'!B22)</f>
-        <v>Prototyping</v>
-      </c>
-      <c r="C19" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C19" s="27">
         <f>('Self-Assessment'!C22)</f>
-        <v>Prototyping a service or product involves exploring, testing and sharing different concepts before committing to the final design.</v>
-      </c>
-      <c r="D19" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D19" s="28">
         <f>('Self-Assessment'!D22)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E19" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E19" s="29">
         <f>('Self-Assessment'!E22)</f>
-        <v>You can:
-- approach prototyping as a team activity, actively soliciting prototypes and testing with others
-- establish design patterns and iterate them
-- use a variety of prototyping methods and choose the most appropriate</v>
+        <v>0</v>
       </c>
       <c r="F19" s="160"/>
       <c r="G19" s="63">
@@ -3192,22 +2954,21 @@
     </row>
     <row r="20" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="62"/>
-      <c r="B20" s="26" t="str">
+      <c r="B20" s="26">
         <f>('Self-Assessment'!B23)</f>
-        <v>Service support</v>
-      </c>
-      <c r="C20" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C20" s="27">
         <f>('Self-Assessment'!C23)</f>
-        <v>Service support involves fixing service faults and maintaining the underlying infrastructure, ensuring processes are in place to keep the service running efficiently.</v>
-      </c>
-      <c r="D20" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D20" s="28">
         <f>('Self-Assessment'!D23)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E20" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
         <f>('Self-Assessment'!E23)</f>
-        <v>You can:
-- identify, locate and fix faults</v>
+        <v>0</v>
       </c>
       <c r="F20" s="160"/>
       <c r="G20" s="63">
@@ -3241,24 +3002,21 @@
     </row>
     <row r="21" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62"/>
-      <c r="B21" s="26" t="str">
+      <c r="B21" s="26">
         <f>('Self-Assessment'!B24)</f>
-        <v>Systems design</v>
-      </c>
-      <c r="C21" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C21" s="27">
         <f>('Self-Assessment'!C24)</f>
-        <v>Systems design involves creating the specification and design of systems to meet defined business needs.</v>
-      </c>
-      <c r="D21" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D21" s="28">
         <f>('Self-Assessment'!D24)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E21" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E21" s="29">
         <f>('Self-Assessment'!E24)</f>
-        <v>You can:
-- design systems characterised by medium levels of risk, impact, and business or technical complexity
-- select appropriate design standards, methods and tools, and ensure they are applied effectively
-- review the systems designs of others to ensure the selection of appropriate technology, efficient use of resources and integration of multiple systems and technology</v>
+        <v>0</v>
       </c>
       <c r="F21" s="160"/>
       <c r="G21" s="63">
@@ -3292,24 +3050,21 @@
     </row>
     <row r="22" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="62"/>
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="26">
         <f>('Self-Assessment'!B25)</f>
-        <v>Systems integration</v>
-      </c>
-      <c r="C22" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C22" s="27">
         <f>('Self-Assessment'!C25)</f>
-        <v>Systems integration involves identifying points of connection between different systems and processes, or opportunities to combine them, and designing how the components communicate.</v>
-      </c>
-      <c r="D22" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D22" s="28">
         <f>('Self-Assessment'!D25)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E22" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E22" s="29">
         <f>('Self-Assessment'!E25)</f>
-        <v>You can:
-- define the integration build
-- co-ordinate build activities across systems
-- understand how to undertake and support integration testing activities</v>
+        <v>0</v>
       </c>
       <c r="F22" s="160"/>
       <c r="G22" s="63">
@@ -3343,26 +3098,21 @@
     </row>
     <row r="23" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="62"/>
-      <c r="B23" s="26" t="str">
+      <c r="B23" s="26">
         <f>('Self-Assessment'!B26)</f>
-        <v>User focus</v>
-      </c>
-      <c r="C23" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C23" s="27">
         <f>('Self-Assessment'!C26)</f>
-        <v>User focus involves understanding the user needs to develop a detailed understanding of the problems that need to be solved.</v>
-      </c>
-      <c r="D23" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D23" s="28">
         <f>('Self-Assessment'!D26)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E23" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29">
         <f>('Self-Assessment'!E26)</f>
-        <v>You can:
-- collaborate with user researchers and can represent users internally
-- explain the difference between user needs and the desires of the user
-- champion user research to focus on all users
-- prioritise and define approaches to understand the user story, guiding others in doing so
-- offer recommendations on the best tools and methods to use</v>
+        <v>0</v>
       </c>
       <c r="F23" s="160"/>
       <c r="G23" s="63">
@@ -3425,7 +3175,7 @@
       <c r="J25" s="175"/>
       <c r="K25" s="174"/>
       <c r="L25" s="176" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="M25" s="173"/>
       <c r="N25" s="175"/>
@@ -3445,7 +3195,7 @@
       <c r="J26" s="175"/>
       <c r="K26" s="174"/>
       <c r="L26" s="185" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="M26" s="186"/>
       <c r="N26" s="186"/>
@@ -3532,7 +3282,7 @@
       <c r="E31" s="62"/>
       <c r="F31" s="64"/>
       <c r="G31" s="157" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="H31" s="67" t="str">
         <f>IFERROR(ROUNDUP(AVERAGE($H$14:$H$23),2)," ")</f>
@@ -3542,7 +3292,7 @@
       <c r="J31" s="48"/>
       <c r="K31" s="64"/>
       <c r="L31" s="157" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="M31" s="68" t="str">
         <f>IFERROR(ROUNDUP(AVERAGE($M$14:$M$23),2)," ")</f>
@@ -3560,7 +3310,7 @@
       <c r="E32" s="62"/>
       <c r="F32" s="64"/>
       <c r="G32" s="157" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="H32" s="67" t="str">
         <f>'Proficiency Calculations'!E16</f>
@@ -3570,7 +3320,7 @@
       <c r="J32" s="48"/>
       <c r="K32" s="64"/>
       <c r="L32" s="157" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="M32" s="68" t="str">
         <f>'Proficiency Calculations'!E18</f>
@@ -3588,7 +3338,7 @@
       <c r="E33" s="62"/>
       <c r="F33" s="64"/>
       <c r="G33" s="157" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="H33" s="67" t="str">
         <f>'Proficiency Calculations'!H16</f>
@@ -3598,7 +3348,7 @@
       <c r="J33" s="48"/>
       <c r="K33" s="64"/>
       <c r="L33" s="157" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="M33" s="68" t="str">
         <f>'Proficiency Calculations'!H18</f>
@@ -3616,7 +3366,7 @@
       <c r="E34" s="62"/>
       <c r="F34" s="64"/>
       <c r="G34" s="157" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="H34" s="67" t="str">
         <f>'Proficiency Calculations'!I16</f>
@@ -3626,7 +3376,7 @@
       <c r="J34" s="48"/>
       <c r="K34" s="64"/>
       <c r="L34" s="157" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="M34" s="68" t="str">
         <f>'Proficiency Calculations'!I18</f>
@@ -3644,7 +3394,7 @@
       <c r="E35" s="62"/>
       <c r="F35" s="64"/>
       <c r="G35" s="69" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="H35" s="70" t="str">
         <f>'Proficiency Calculations'!J16</f>
@@ -3654,7 +3404,7 @@
       <c r="J35" s="48"/>
       <c r="K35" s="64"/>
       <c r="L35" s="69" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="M35" s="71" t="str">
         <f>'Proficiency Calculations'!J18</f>
@@ -3672,7 +3422,7 @@
       <c r="E36" s="62"/>
       <c r="F36" s="64"/>
       <c r="G36" s="69" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="H36" s="70" t="str">
         <f>'Proficiency Calculations'!L16</f>
@@ -3682,7 +3432,7 @@
       <c r="J36" s="48"/>
       <c r="K36" s="64"/>
       <c r="L36" s="69" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="M36" s="71" t="str">
         <f>'Proficiency Calculations'!L18</f>
@@ -3705,7 +3455,7 @@
       <c r="J37" s="48"/>
       <c r="K37" s="64"/>
       <c r="L37" s="69" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="M37" s="72" t="str">
         <f>'Proficiency Calculations'!D20</f>
@@ -3875,7 +3625,7 @@
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="74"/>
       <c r="B4" s="73" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="73"/>
@@ -3900,9 +3650,9 @@
       <c r="F5" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="80" t="str">
+      <c r="G5" s="80">
         <f>'Self-Assessment'!C11</f>
-        <v>Software Development</v>
+        <v>0</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="73"/>
@@ -3921,11 +3671,11 @@
       <c r="D6" s="162"/>
       <c r="E6" s="73"/>
       <c r="F6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="81" t="str">
+        <v>14</v>
+      </c>
+      <c r="G6" s="81">
         <f>'Self-Assessment'!C12</f>
-        <v>Software Developer</v>
+        <v>0</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="73"/>
@@ -3941,11 +3691,11 @@
       <c r="D7" s="76"/>
       <c r="E7" s="73"/>
       <c r="F7" s="152" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="82" t="str">
+        <v>16</v>
+      </c>
+      <c r="G7" s="82">
         <f>'Self-Assessment'!C13</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="H7" s="153"/>
       <c r="I7" s="73"/>
@@ -3973,31 +3723,31 @@
       <c r="A9" s="74"/>
       <c r="B9" s="75"/>
       <c r="C9" s="157" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="D9" s="157" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E9" s="83" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="F9" s="83" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="G9" s="157" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="H9" s="157" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="I9" s="83" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="J9" s="157" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="K9" s="157" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="L9" s="73"/>
       <c r="M9" s="73"/>
@@ -4026,10 +3776,10 @@
         <v>3</v>
       </c>
       <c r="H10" s="86" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="I10" s="86" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="J10" s="86">
         <v>5</v>
@@ -4055,7 +3805,7 @@
         <v/>
       </c>
       <c r="E11" s="89" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="F11" s="88">
         <v>2.7</v>
@@ -4064,10 +3814,10 @@
         <v>2.99</v>
       </c>
       <c r="H11" s="89" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="I11" s="89" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="J11" s="89">
         <v>4</v>
@@ -4093,7 +3843,7 @@
         <v/>
       </c>
       <c r="E12" s="89" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="F12" s="88">
         <v>2</v>
@@ -4102,10 +3852,10 @@
         <v>2.69</v>
       </c>
       <c r="H12" s="89" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="I12" s="89" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="J12" s="89">
         <v>3</v>
@@ -4131,7 +3881,7 @@
         <v/>
       </c>
       <c r="E13" s="89" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="F13" s="88">
         <v>1.6</v>
@@ -4140,10 +3890,10 @@
         <v>1.99</v>
       </c>
       <c r="H13" s="89" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="I13" s="89" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="J13" s="89">
         <v>2</v>
@@ -4169,7 +3919,7 @@
         <v/>
       </c>
       <c r="E14" s="91" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="F14" s="90">
         <v>1</v>
@@ -4178,10 +3928,10 @@
         <v>1.59</v>
       </c>
       <c r="H14" s="92" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="I14" s="92" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="J14" s="92">
         <v>1</v>
@@ -4210,7 +3960,7 @@
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="24" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="C16" s="93" t="str">
         <f>Evaluation!H31</f>
@@ -4269,7 +4019,7 @@
     <row r="18" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="24" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="C18" s="94"/>
       <c r="D18" s="98" t="str">
@@ -4329,7 +4079,7 @@
       <c r="A20" s="74"/>
       <c r="B20" s="74"/>
       <c r="C20" s="69" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="D20" s="72" t="str">
         <f>IFERROR(D18-C16," ")</f>
@@ -4416,54 +4166,54 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="100" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B1" s="101" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C1" s="101" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D1" s="101" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="B2" s="103" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="C2" s="103">
         <v>1</v>
       </c>
       <c r="D2" s="103" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="104"/>
       <c r="B3" s="105" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="C3" s="105">
         <v>2</v>
       </c>
       <c r="D3" s="105" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="106" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="C4" s="106">
         <v>3</v>
       </c>
       <c r="D4" s="105" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4471,7 +4221,7 @@
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
       <c r="D5" s="105" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4479,7 +4229,7 @@
       <c r="B6" s="104"/>
       <c r="C6" s="104"/>
       <c r="D6" s="106" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4517,13 +4267,13 @@
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="163"/>
       <c r="B1" s="108" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="C1" s="109"/>
       <c r="D1" s="110"/>
       <c r="E1" s="111"/>
       <c r="F1" s="112" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="G1" s="113"/>
       <c r="H1" s="113"/>
@@ -4543,56 +4293,56 @@
         <v>4</v>
       </c>
       <c r="B2" s="114" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C2" s="166" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="D2" s="166" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="E2" s="167" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="168" t="str">
+        <v>98</v>
+      </c>
+      <c r="F2" s="168">
         <f>'Self-Assessment'!$B$17</f>
-        <v>Availability and capacity management</v>
-      </c>
-      <c r="G2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="G2" s="168">
         <f>'Self-Assessment'!$B$18</f>
-        <v>Development process optimisation</v>
-      </c>
-      <c r="H2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="H2" s="168">
         <f>'Self-Assessment'!$B$19</f>
-        <v>Information security</v>
-      </c>
-      <c r="I2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="I2" s="168">
         <f>'Self-Assessment'!$B$20</f>
-        <v>Modern standards approach</v>
-      </c>
-      <c r="J2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="J2" s="168">
         <f>'Self-Assessment'!$B$21</f>
-        <v>Programming and build (software engineering)</v>
-      </c>
-      <c r="K2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="K2" s="168">
         <f>'Self-Assessment'!$B$22</f>
-        <v>Prototyping</v>
-      </c>
-      <c r="L2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="L2" s="168">
         <f>'Self-Assessment'!$B$23</f>
-        <v>Service support</v>
-      </c>
-      <c r="M2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="M2" s="168">
         <f>'Self-Assessment'!$B$24</f>
-        <v>Systems design</v>
-      </c>
-      <c r="N2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="N2" s="168">
         <f>'Self-Assessment'!$B$25</f>
-        <v>Systems integration</v>
-      </c>
-      <c r="O2" s="168" t="str">
+        <v>0</v>
+      </c>
+      <c r="O2" s="168">
         <f>'Self-Assessment'!$B$26</f>
-        <v>User focus</v>
+        <v>0</v>
       </c>
       <c r="P2" s="168" t="e">
         <f>'Self-Assessment'!#REF!</f>
@@ -4603,7 +4353,7 @@
         <v>#REF!</v>
       </c>
       <c r="R2" s="169" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="S2" s="115"/>
       <c r="T2" s="115"/>
@@ -4619,20 +4369,20 @@
         <f>'Self-Assessment'!$E$8</f>
         <v>0</v>
       </c>
-      <c r="B3" s="104" t="str">
+      <c r="B3" s="104">
         <f>'Self-Assessment'!$C$11</f>
-        <v>Software Development</v>
-      </c>
-      <c r="C3" s="104" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="104">
         <f>'Self-Assessment'!$C$12</f>
-        <v>Software Developer</v>
-      </c>
-      <c r="D3" s="104" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="104">
         <f>'Self-Assessment'!A3_RoleLevel</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="E3" s="116" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="F3" s="104" t="str">
         <f>Evaluation!$H$14</f>
@@ -4692,20 +4442,20 @@
         <f>'Self-Assessment'!$E$8</f>
         <v>0</v>
       </c>
-      <c r="B4" s="104" t="str">
+      <c r="B4" s="104">
         <f>'Self-Assessment'!$C$11</f>
-        <v>Software Development</v>
-      </c>
-      <c r="C4" s="104" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="104">
         <f>'Self-Assessment'!$C$12</f>
-        <v>Software Developer</v>
-      </c>
-      <c r="D4" s="104" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" s="104">
         <f>'Self-Assessment'!A3_RoleLevel</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="F4" s="104" t="str">
         <f>Evaluation!$M$14</f>
@@ -5852,12 +5602,12 @@
     <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="37"/>
       <c r="B4" s="41" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="49"/>
       <c r="E4" s="155" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -5918,13 +5668,13 @@
       <c r="B7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="16" t="str">
+      <c r="C7" s="16">
         <f>('Self-Assessment'!C11)</f>
-        <v>Software Development</v>
+        <v>0</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="155" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="54"/>
@@ -5936,18 +5686,18 @@
       <c r="M7" s="54"/>
       <c r="N7" s="54"/>
       <c r="O7" s="157" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="P7" s="39"/>
     </row>
     <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
       <c r="B8" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="str">
+        <v>14</v>
+      </c>
+      <c r="C8" s="19">
         <f>('Self-Assessment'!C12)</f>
-        <v>Software Developer</v>
+        <v>0</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="158"/>
@@ -5961,18 +5711,18 @@
       <c r="M8" s="56"/>
       <c r="N8" s="56"/>
       <c r="O8" s="151" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="42"/>
       <c r="B9" s="159" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="153" t="str">
+        <v>16</v>
+      </c>
+      <c r="C9" s="153">
         <f>('Self-Assessment'!C13)</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="57">
@@ -6033,7 +5783,7 @@
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="180" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12" s="181"/>
       <c r="D12" s="181"/>
@@ -6042,12 +5792,12 @@
       <c r="G12" s="184"/>
       <c r="H12" s="181"/>
       <c r="I12" s="183" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J12" s="182"/>
       <c r="K12" s="42"/>
       <c r="L12" s="180" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="M12" s="181"/>
       <c r="N12" s="181"/>
@@ -6057,65 +5807,62 @@
     <row r="13" spans="1:16" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="B13" s="22" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" s="160"/>
       <c r="G13" s="61" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="K13" s="42"/>
       <c r="L13" s="22" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="P13" s="42"/>
     </row>
     <row r="14" spans="1:16" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
-      <c r="B14" s="26" t="str">
+      <c r="B14" s="26">
         <f>('Self-Assessment'!B17)</f>
-        <v>Availability and capacity management</v>
-      </c>
-      <c r="C14" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C14" s="27">
         <f>('Self-Assessment'!C17)</f>
-        <v>Availability and capacity management involves ensuring services are available with as little down-time or disruption as possible, whilst making sure we have sufficient resources to support emerging business needs.</v>
-      </c>
-      <c r="D14" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28">
         <f>('Self-Assessment'!D17)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E14" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E14" s="29">
         <f>('Self-Assessment'!E17)</f>
-        <v>You can:
-- ensure the correct implementation of standards and procedures
-- identify capacity issues, and stipulate and instigate the required changes
-initiate remedial action</v>
+        <v>0</v>
       </c>
       <c r="F14" s="160"/>
       <c r="G14" s="63">
@@ -6155,25 +5902,21 @@
     </row>
     <row r="15" spans="1:16" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="62"/>
-      <c r="B15" s="26" t="str">
+      <c r="B15" s="26">
         <f>('Self-Assessment'!B18)</f>
-        <v>Development process optimisation</v>
-      </c>
-      <c r="C15" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C15" s="27">
         <f>('Self-Assessment'!C18)</f>
-        <v>Process optimisation involves ensuring your processes are accurately defined and capture the most efficient way to complete a task by monitoring modified procedures.</v>
-      </c>
-      <c r="D15" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28">
         <f>('Self-Assessment'!D18)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E15" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
         <f>('Self-Assessment'!E18)</f>
-        <v>You can:
-- analyse current processes
-- identify and implement opportunities to optimise processes
-- lead and develop a team of experts to deliver service improvements
-- help to evaluate and establish requirements for the implementation of changes by setting policy and standards</v>
+        <v>0</v>
       </c>
       <c r="F15" s="160"/>
       <c r="G15" s="63">
@@ -6213,23 +5956,21 @@
     </row>
     <row r="16" spans="1:16" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="62"/>
-      <c r="B16" s="26" t="str">
+      <c r="B16" s="26">
         <f>('Self-Assessment'!B19)</f>
-        <v>Information security</v>
-      </c>
-      <c r="C16" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27">
         <f>('Self-Assessment'!C19)</f>
-        <v>Information security involves maintaining the security, confidentiality and integrity of information.</v>
-      </c>
-      <c r="D16" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28">
         <f>('Self-Assessment'!D19)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E16" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E16" s="29">
         <f>('Self-Assessment'!E19)</f>
-        <v>You can:
-- understand information security
-- design solutions and services with security controls embedded, specifically engineered with mitigation of security threats as a core feature</v>
+        <v>0</v>
       </c>
       <c r="F16" s="160"/>
       <c r="G16" s="63">
@@ -6269,23 +6010,21 @@
     </row>
     <row r="17" spans="1:16" ht="291" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62"/>
-      <c r="B17" s="26" t="str">
+      <c r="B17" s="26">
         <f>('Self-Assessment'!B20)</f>
-        <v>Modern standards approach</v>
-      </c>
-      <c r="C17" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C17" s="27">
         <f>('Self-Assessment'!C20)</f>
-        <v>Modern development standards involves using the latest technologies and best practices to improve the quality of the software development process.</v>
-      </c>
-      <c r="D17" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D17" s="28">
         <f>('Self-Assessment'!D20)</f>
-        <v>Expert</v>
-      </c>
-      <c r="E17" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E17" s="29">
         <f>('Self-Assessment'!E20)</f>
-        <v>You can:
-- demonstrate a strong understanding of the most appropriate modern standards and practices, and how they are applied
-- coach and guide others in these standards</v>
+        <v>0</v>
       </c>
       <c r="F17" s="160"/>
       <c r="G17" s="63">
@@ -6325,23 +6064,21 @@
     </row>
     <row r="18" spans="1:16" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
-      <c r="B18" s="26" t="str">
+      <c r="B18" s="26">
         <f>('Self-Assessment'!B21)</f>
-        <v>Programming and build (software engineering)</v>
-      </c>
-      <c r="C18" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C18" s="27">
         <f>('Self-Assessment'!C21)</f>
-        <v>You can use agreed security standards and specifications to design, create, test and document new or amended software.</v>
-      </c>
-      <c r="D18" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D18" s="28">
         <f>('Self-Assessment'!D21)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E18" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E18" s="29">
         <f>('Self-Assessment'!E21)</f>
-        <v>You can:
-- collaborate with others when necessary to review specifications
-- use the agreed specifications to design, code, test and document programs or scripts of medium-to-high complexity, using the right standards and tools</v>
+        <v>0</v>
       </c>
       <c r="F18" s="160"/>
       <c r="G18" s="63">
@@ -6381,24 +6118,21 @@
     </row>
     <row r="19" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62"/>
-      <c r="B19" s="26" t="str">
+      <c r="B19" s="26">
         <f>('Self-Assessment'!B22)</f>
-        <v>Prototyping</v>
-      </c>
-      <c r="C19" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C19" s="27">
         <f>('Self-Assessment'!C22)</f>
-        <v>Prototyping a service or product involves exploring, testing and sharing different concepts before committing to the final design.</v>
-      </c>
-      <c r="D19" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D19" s="28">
         <f>('Self-Assessment'!D22)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E19" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E19" s="29">
         <f>('Self-Assessment'!E22)</f>
-        <v>You can:
-- approach prototyping as a team activity, actively soliciting prototypes and testing with others
-- establish design patterns and iterate them
-- use a variety of prototyping methods and choose the most appropriate</v>
+        <v>0</v>
       </c>
       <c r="F19" s="160"/>
       <c r="G19" s="63">
@@ -6438,22 +6172,21 @@
     </row>
     <row r="20" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="62"/>
-      <c r="B20" s="26" t="str">
+      <c r="B20" s="26">
         <f>('Self-Assessment'!B23)</f>
-        <v>Service support</v>
-      </c>
-      <c r="C20" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C20" s="27">
         <f>('Self-Assessment'!C23)</f>
-        <v>Service support involves fixing service faults and maintaining the underlying infrastructure, ensuring processes are in place to keep the service running efficiently.</v>
-      </c>
-      <c r="D20" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D20" s="28">
         <f>('Self-Assessment'!D23)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E20" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
         <f>('Self-Assessment'!E23)</f>
-        <v>You can:
-- identify, locate and fix faults</v>
+        <v>0</v>
       </c>
       <c r="F20" s="160"/>
       <c r="G20" s="63">
@@ -6493,24 +6226,21 @@
     </row>
     <row r="21" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62"/>
-      <c r="B21" s="26" t="str">
+      <c r="B21" s="26">
         <f>('Self-Assessment'!B24)</f>
-        <v>Systems design</v>
-      </c>
-      <c r="C21" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C21" s="27">
         <f>('Self-Assessment'!C24)</f>
-        <v>Systems design involves creating the specification and design of systems to meet defined business needs.</v>
-      </c>
-      <c r="D21" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D21" s="28">
         <f>('Self-Assessment'!D24)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E21" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E21" s="29">
         <f>('Self-Assessment'!E24)</f>
-        <v>You can:
-- design systems characterised by medium levels of risk, impact, and business or technical complexity
-- select appropriate design standards, methods and tools, and ensure they are applied effectively
-- review the systems designs of others to ensure the selection of appropriate technology, efficient use of resources and integration of multiple systems and technology</v>
+        <v>0</v>
       </c>
       <c r="F21" s="160"/>
       <c r="G21" s="63">
@@ -6550,24 +6280,21 @@
     </row>
     <row r="22" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="62"/>
-      <c r="B22" s="26" t="str">
+      <c r="B22" s="26">
         <f>('Self-Assessment'!B25)</f>
-        <v>Systems integration</v>
-      </c>
-      <c r="C22" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C22" s="27">
         <f>('Self-Assessment'!C25)</f>
-        <v>Systems integration involves identifying points of connection between different systems and processes, or opportunities to combine them, and designing how the components communicate.</v>
-      </c>
-      <c r="D22" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D22" s="28">
         <f>('Self-Assessment'!D25)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E22" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E22" s="29">
         <f>('Self-Assessment'!E25)</f>
-        <v>You can:
-- define the integration build
-- co-ordinate build activities across systems
-- understand how to undertake and support integration testing activities</v>
+        <v>0</v>
       </c>
       <c r="F22" s="160"/>
       <c r="G22" s="63">
@@ -6607,26 +6334,21 @@
     </row>
     <row r="23" spans="1:16" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="62"/>
-      <c r="B23" s="26" t="str">
+      <c r="B23" s="26">
         <f>('Self-Assessment'!B26)</f>
-        <v>User focus</v>
-      </c>
-      <c r="C23" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C23" s="27">
         <f>('Self-Assessment'!C26)</f>
-        <v>User focus involves understanding the user needs to develop a detailed understanding of the problems that need to be solved.</v>
-      </c>
-      <c r="D23" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="D23" s="28">
         <f>('Self-Assessment'!D26)</f>
-        <v>Practitioner</v>
-      </c>
-      <c r="E23" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29">
         <f>('Self-Assessment'!E26)</f>
-        <v>You can:
-- collaborate with user researchers and can represent users internally
-- explain the difference between user needs and the desires of the user
-- champion user research to focus on all users
-- prioritise and define approaches to understand the user story, guiding others in doing so
-- offer recommendations on the best tools and methods to use</v>
+        <v>0</v>
       </c>
       <c r="F23" s="160"/>
       <c r="G23" s="63">
@@ -8267,7 +7989,7 @@
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="118"/>
       <c r="B2" s="121" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121"/>
@@ -8325,10 +8047,10 @@
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="118"/>
       <c r="B4" s="121" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="C4" s="155" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D4" s="125"/>
       <c r="E4" s="120"/>
@@ -8448,9 +8170,9 @@
       <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="16" t="str">
+      <c r="C8" s="16">
         <f>'Self-Assessment'!C11</f>
-        <v>Software Development</v>
+        <v>0</v>
       </c>
       <c r="D8" s="127"/>
       <c r="E8" s="120"/>
@@ -8479,11 +8201,11 @@
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="127"/>
       <c r="B9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="19" t="str">
+        <v>14</v>
+      </c>
+      <c r="C9" s="19">
         <f>'Self-Assessment'!C12</f>
-        <v>Software Developer</v>
+        <v>0</v>
       </c>
       <c r="D9" s="124"/>
       <c r="E9" s="120"/>
@@ -8512,11 +8234,11 @@
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="127"/>
       <c r="B10" s="152" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="153" t="str">
+        <v>16</v>
+      </c>
+      <c r="C10" s="153">
         <f>'Self-Assessment'!C13</f>
-        <v>Lead Developer (Management)</v>
+        <v>0</v>
       </c>
       <c r="D10" s="124"/>
       <c r="E10" s="120"/>
@@ -8573,7 +8295,7 @@
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="128"/>
       <c r="B12" s="129" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C12" s="130"/>
       <c r="D12" s="128"/>
@@ -8631,7 +8353,7 @@
     <row r="14" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="133"/>
       <c r="B14" s="194" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="C14" s="195"/>
       <c r="D14" s="133"/>
@@ -8689,7 +8411,7 @@
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="133"/>
       <c r="B16" s="134" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="C16" s="135" t="str">
         <f>Evaluation!H31</f>
@@ -8750,7 +8472,7 @@
     <row r="18" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="138"/>
       <c r="B18" s="196" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="C18" s="195"/>
       <c r="D18" s="138"/>
@@ -8808,7 +8530,7 @@
     <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="128"/>
       <c r="B20" s="140" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="C20" s="141" t="str">
         <f>Evaluation!M31</f>
@@ -8869,7 +8591,7 @@
     <row r="22" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="144"/>
       <c r="B22" s="197" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C22" s="195"/>
       <c r="D22" s="144"/>
@@ -8927,7 +8649,7 @@
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="128"/>
       <c r="B24" s="145" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C24" s="146"/>
       <c r="D24" s="128"/>
@@ -36299,6 +36021,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <QA xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330" xsi:nil="true"/>
+    <Redaction_x002b_Addboxforevaluatorfeedback xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020F8048989A69440AAAC4510BE85C76B" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4c3fa747d40dc231885262c336faa7c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="87f18c74-00e5-43bc-a7dc-ee7546fc9330" xmlns:ns3="336332ac-cff5-4241-a26c-c74692bc7fe4" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="085525847c639d1cb16fd3e02c51a25e" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36615,31 +36361,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC36054-6628-4DC6-A40E-7EA55AF8082C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <QA xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330" xsi:nil="true"/>
-    <Redaction_x002b_Addboxforevaluatorfeedback xmlns="87f18c74-00e5-43bc-a7dc-ee7546fc9330" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35059DB-C5F5-4FB3-9E65-FEB4FAB0B5E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87f18c74-00e5-43bc-a7dc-ee7546fc9330"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="336332ac-cff5-4241-a26c-c74692bc7fe4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64DA766B-C9C1-41AE-AFE3-C78079235F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36660,33 +36409,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC36054-6628-4DC6-A40E-7EA55AF8082C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B35059DB-C5F5-4FB3-9E65-FEB4FAB0B5E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87f18c74-00e5-43bc-a7dc-ee7546fc9330"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="336332ac-cff5-4241-a26c-c74692bc7fe4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" removed="0"/>

</xml_diff>